<commit_message>
Erstellen des Login für Android
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Als Mitarbeiter der Personalabteilung möchte ich einen Dienstplan generieren lassen.</t>
+  </si>
+  <si>
+    <t>Als Geschäftsleiter möchte ich Urlaubsanträge einsehen können</t>
+  </si>
+  <si>
+    <t>Als Mitarbeiter möchte ich mich über mein Android smartphone einloggen</t>
   </si>
 </sst>
 </file>
@@ -208,7 +214,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -259,26 +265,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -323,10 +309,13 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$A$34:$A$45</c:f>
+              <c:f>Tabelle1!$B$35:$B$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>320</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -336,7 +325,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$D$8</c:f>
+              <c:f>Tabelle1!$E$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -357,7 +346,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$D$8</c:f>
+              <c:f>Tabelle1!$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -378,11 +367,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="292262864"/>
-        <c:axId val="292263256"/>
+        <c:axId val="68469504"/>
+        <c:axId val="68471040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292262864"/>
+        <c:axId val="68469504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -421,10 +410,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292263256"/>
+        <c:crossAx val="68471040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -432,7 +421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292263256"/>
+        <c:axId val="68471040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -481,10 +470,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292262864"/>
+        <c:crossAx val="68469504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -528,7 +517,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1088,15 +1077,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>4762</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>309562</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1377,9 +1366,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1417,9 +1406,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1454,7 +1443,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1489,7 +1478,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1663,341 +1652,381 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D33"/>
+  <dimension ref="A2:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="126.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="126.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="str">
-        <f>VLOOKUP(A3,[1]Tabelle1!B:F,2,0)</f>
+      <c r="C3" s="1" t="str">
+        <f>VLOOKUP(B3,[1]Tabelle1!B:F,2,0)</f>
         <v>Als Mitarbeiter möchte ich mich einloggen können</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="str">
-        <f>VLOOKUP(A4,[1]Tabelle1!B:F,2,0)</f>
+      <c r="C4" s="1" t="str">
+        <f>VLOOKUP(B4,[1]Tabelle1!B:F,2,0)</f>
         <v>Als Personalleiter möchte ich mich einloggen können</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <v>30</v>
       </c>
-      <c r="B5" s="1" t="str">
-        <f>VLOOKUP(A5,[1]Tabelle1!B:F,2,0)</f>
+      <c r="C5" s="1" t="str">
+        <f>VLOOKUP(B5,[1]Tabelle1!B:F,2,0)</f>
         <v>Als Mitarbeiter der Personalabteilung möchte ich neue Mitarbeiter anlegen können</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>40</v>
       </c>
-      <c r="B6" s="1" t="str">
-        <f>VLOOKUP(A6,[1]Tabelle1!B:F,2,0)</f>
+      <c r="C6" s="1" t="str">
+        <f>VLOOKUP(B6,[1]Tabelle1!B:F,2,0)</f>
         <v>Als Mitarbeiter der Personalabteilung möchte ich Mitarbeiter verwalten (ändern + löschen) können</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
         <v>50</v>
       </c>
-      <c r="B7" s="1" t="str">
-        <f>VLOOKUP(A7,[1]Tabelle1!B:F,2,0)</f>
+      <c r="C7" s="1" t="str">
+        <f>VLOOKUP(B7,[1]Tabelle1!B:F,2,0)</f>
         <v>Als Mitarbeiter der Personalabteilung  möchte ich Mitarbeiter suchen können</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>1</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D8">
-        <f>D3+D4+D5+D6+D7</f>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <f>E3+E4+E5+E6+E7</f>
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9">
         <v>60</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10">
         <v>70</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11">
         <v>80</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12">
         <v>90</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>100</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>310</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15">
         <v>110</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16">
         <v>120</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17">
         <v>130</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18">
         <v>140</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19">
         <v>150</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20">
         <v>160</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21">
         <v>170</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22">
         <v>180</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
         <v>190</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
         <v>200</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25">
         <v>210</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26">
         <v>220</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27">
         <v>230</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28">
         <v>240</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29">
         <v>250</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30">
         <v>260</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31">
         <v>270</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B32">
         <v>280</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33">
         <v>290</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34">
         <v>300</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>320</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3">
+  <conditionalFormatting sqref="C3">
     <cfRule type="expression" dxfId="4" priority="5">
       <formula>"MOD($A2:$A,10)"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4">
+  <conditionalFormatting sqref="C4">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>"MOD($A2:$A,10)"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
+  <conditionalFormatting sqref="C5">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>"MOD($A2:$A,10)"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
+  <conditionalFormatting sqref="C6">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>"MOD($A2:$A,10)"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
+  <conditionalFormatting sqref="C7">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>"MOD($A2:$A,10)"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>